<commit_message>
Correzione colonna mancante su file excel
</commit_message>
<xml_diff>
--- a/TISDeroga2020/TracciatoXLSX/XLSX_TIS_DEROGA_2020.xlsx
+++ b/TISDeroga2020/TracciatoXLSX/XLSX_TIS_DEROGA_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Repositories\tis_rendicontazione_deroga\TISDeroga2020\TracciatoXLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE07A08-1026-4D68-8F3B-271A41674BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EAF7BD-4730-45A9-A0B5-8D436C45D5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="483" xr2:uid="{C62F197E-4834-1546-9B8C-4BDFB4210C62}"/>
+    <workbookView xWindow="6330" yWindow="2430" windowWidth="21600" windowHeight="11505" tabRatio="483" activeTab="1" xr2:uid="{C62F197E-4834-1546-9B8C-4BDFB4210C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Istanze" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="78">
   <si>
     <t>identificativoPratica</t>
   </si>
@@ -210,6 +210,72 @@
   </si>
   <si>
     <t>percentualeSgraviAliquotaContributivaPrevidenziale</t>
+  </si>
+  <si>
+    <t>12345678901-H501</t>
+  </si>
+  <si>
+    <t>RSSMRA70H14H501V</t>
+  </si>
+  <si>
+    <t>Rossi</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>12345678901-G273</t>
+  </si>
+  <si>
+    <t>VRDGPP70H14G273B</t>
+  </si>
+  <si>
+    <t>Verdini</t>
+  </si>
+  <si>
+    <t>Giuseppe</t>
+  </si>
+  <si>
+    <t>98765432101-F205</t>
+  </si>
+  <si>
+    <t>BNCMRR70H14G273B</t>
+  </si>
+  <si>
+    <t>Bianchi</t>
+  </si>
+  <si>
+    <t>Mariolina</t>
+  </si>
+  <si>
+    <t>APL DI ESEMPIO SPA</t>
+  </si>
+  <si>
+    <t>UTILIZZATORE 1</t>
+  </si>
+  <si>
+    <t>12345678901</t>
+  </si>
+  <si>
+    <t>42.54.41</t>
+  </si>
+  <si>
+    <t>H501</t>
+  </si>
+  <si>
+    <t>G273</t>
+  </si>
+  <si>
+    <t>UTILIZZATORE 2</t>
+  </si>
+  <si>
+    <t>66557744110</t>
+  </si>
+  <si>
+    <t>24.25.21</t>
+  </si>
+  <si>
+    <t>F205</t>
   </si>
 </sst>
 </file>
@@ -245,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -258,11 +324,24 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -585,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7CC479-9EB7-1D4B-A1C1-E99C9EBFB207}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -667,16 +746,178 @@
         <v>49</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="2">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="R3" s="5"/>
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="2">
+        <v>7</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="5">
+        <v>43884</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="R4" s="5"/>
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="2">
+        <v>6</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="5">
+        <v>43915</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="lsCkfPiVX2CEoBNuoOJ3ddp2pO4Vs/p73P4JI2/4QVyF9ny0Ww9jYOyIxX4YB8M17LIJAnuGwVfighkoAOlvZg==" saltValue="WdWMaLUMnV7TiYTm72zGOg==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
   <autoFilter ref="A1:S1" xr:uid="{369444C7-00C3-41FE-89D1-20E39C1266F3}"/>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A1 A5:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A4">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="11">
@@ -718,37 +959,37 @@
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:K1048576</xm:sqref>
+          <xm:sqref>J5:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Settore di Riferimento" error="Indicare il settore di Riferimento dell'utilizzatore (ED = Edile, NE = Non Edile)" promptTitle="Settore di Riferimento" prompt="Indicare il settore di Riferimento dell'utilizzatore (ED = Edile, NE = Non Edile)" xr:uid="{A19420F9-B38C-44B3-BC72-E03CCF4E7014}">
           <x14:formula1>
             <xm:f>Tipologiche!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:K1048576</xm:sqref>
+          <xm:sqref>I5:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Autocertificazione Emergenza C19" error="Autocertificazione delle ApL di ricorso al TIS in deroga per cause direttamente o indirettamente riconducibili all'emergenza COVID 19" promptTitle="Autocertificazione Emergenza C19" prompt="Autocertificazione delle ApL di ricorso al TIS in deroga per cause direttamente o indirettamente riconducibili all'emergenza COVID 19" xr:uid="{23FBAEFF-7AE9-4221-9C8C-FC26919B11BF}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O1048576 N2:N1048576</xm:sqref>
+          <xm:sqref>N5:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Soglia Dimensionale Uno" error="L'istanza - sia nelle ipotesi di datore di lavoro pubblico che privato - è relativa ad un numero di lavoratori somministrati fino a 10 (soglia dimensionale 1)" promptTitle="Soglia Dimensionale Uno" prompt="L'istanza - sia nelle ipotesi di datore di lavoro pubblico che privato - è relativa ad un numero di lavoratori somministrati fino a 10 (soglia dimensionale 1)" xr:uid="{C27F54D4-8904-45F0-879D-839E1A9ED2EB}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>P5:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Soglia Dimensionale Due" error="L'istanza è relativa ad imprese senza dipendenti fino ad un massimo di 8 lavoratori somministrati per ciascuna Agenzia interessata (soglia dimensionale 2)" promptTitle="Soglia Dimensionale Due" prompt="L'istanza è relativa ad imprese senza dipendenti fino ad un massimo di 8 lavoratori somministrati per ciascuna Agenzia interessata (soglia dimensionale 2)" xr:uid="{22B6FD49-9D43-4762-BC00-BEF40D28CD7A}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q1048576 S2:S1048576</xm:sqref>
+          <xm:sqref>S5:S1048576 Q5:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribuzione Orario Aziendale" error="Inserire un valore compreso tra 5 e 7" promptTitle="Distribuzione Orario Aziendale" prompt="Inserire un valore compreso tra 5 e 7 per indicare la distribuzione di orario prevalente in azienda" xr:uid="{D3E49FB6-06DC-4E95-A898-B9A946E2EBCD}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1048576</xm:sqref>
+          <xm:sqref>N5:N1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -758,10 +999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2A5F62-5E65-EE42-A866-6CDFA1827C3F}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -776,7 +1017,7 @@
     <col min="8" max="8" width="26.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.875" style="6" customWidth="1"/>
     <col min="12" max="12" width="23.625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="36.875" style="2" bestFit="1" customWidth="1"/>
@@ -861,8 +1102,292 @@
         <v>54</v>
       </c>
     </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1250.52</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>150</v>
+      </c>
+      <c r="M2" s="2">
+        <v>200</v>
+      </c>
+      <c r="N2" s="2">
+        <v>350</v>
+      </c>
+      <c r="O2" s="2">
+        <v>50</v>
+      </c>
+      <c r="P2" s="2">
+        <v>300</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>75</v>
+      </c>
+      <c r="R2" s="2">
+        <v>150</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="2">
+        <v>173.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1250.52</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>120</v>
+      </c>
+      <c r="M3" s="2">
+        <v>180</v>
+      </c>
+      <c r="N3" s="2">
+        <v>150</v>
+      </c>
+      <c r="O3" s="2">
+        <v>200</v>
+      </c>
+      <c r="P3" s="2">
+        <v>300</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>20</v>
+      </c>
+      <c r="R3" s="2">
+        <v>200</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="2">
+        <v>173.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="2">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1560.25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>200</v>
+      </c>
+      <c r="M4" s="2">
+        <v>150</v>
+      </c>
+      <c r="N4" s="2">
+        <v>200</v>
+      </c>
+      <c r="O4" s="2">
+        <v>100</v>
+      </c>
+      <c r="P4" s="2">
+        <v>250</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>100</v>
+      </c>
+      <c r="R4" s="2">
+        <v>168</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" s="2">
+        <v>173.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2">
+        <v>9.69</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1680</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="6">
+        <v>4.12</v>
+      </c>
+      <c r="L5" s="2">
+        <v>250</v>
+      </c>
+      <c r="M5" s="2">
+        <v>180</v>
+      </c>
+      <c r="N5" s="2">
+        <v>300</v>
+      </c>
+      <c r="O5" s="2">
+        <v>150</v>
+      </c>
+      <c r="P5" s="2">
+        <v>300</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>100</v>
+      </c>
+      <c r="R5" s="2">
+        <v>176</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W5" s="2">
+        <v>173.33</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="i2f1oPuoUJYbo4w2FNzvgaAY+RbbAaaUR+9b2OPjGxGlDxIbeJEqjNUgJPWIaBh6OtfXw8Ji8yUh9ZkbJc87rw==" saltValue="x9dmzB58bEs6S1IBXXgw0w==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
   <autoFilter ref="A1:V1" xr:uid="{B1E0D013-8FDE-4AA2-A0C8-EA9D2E0E0052}"/>
   <dataConsolidate/>
   <dataValidations count="14">
@@ -885,34 +1410,34 @@
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Retribuzione TIS Riconosciuta" error="Inserire l'importo della RETRIBUZIONE  TIS riconosciuta (espresso in 2 cifre decimali)" promptTitle="Retribuzione TIS Riconosciuta" prompt="Inserire l'importo della RETRIBUZIONE  TIS riconosciuta (espresso in 2 cifre decimali)" sqref="L2:L1048576" xr:uid="{D4BD6746-985C-49DA-BFF4-75D2C7A378C7}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Retribuzione TIS Riconosciuta" error="Inserire l'importo della RETRIBUZIONE  TIS riconosciuta (espresso in 2 cifre decimali)" promptTitle="Retribuzione TIS Riconosciuta" prompt="Inserire l'importo della RETRIBUZIONE  TIS riconosciuta (espresso in 2 cifre decimali)" sqref="L6:L1048576 L2:L5" xr:uid="{D4BD6746-985C-49DA-BFF4-75D2C7A378C7}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Contribuzione TIS Riconosciuta" error="Inserire l'importo della CONTRIBUZIONE TIS Riconosciuta (espresso in 2 cifre decimali)" promptTitle="Contribuzione TIS Riconosciuta" prompt="Inserire l'importo della CONTRIBUZIONE TIS Riconosciuta (espresso in 2 cifre decimali)" sqref="M2:M1048576" xr:uid="{473EDD48-0FC2-4480-A8CD-51AF57C80278}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Contribuzione TIS Riconosciuta" error="Inserire l'importo della CONTRIBUZIONE TIS Riconosciuta (espresso in 2 cifre decimali)" promptTitle="Contribuzione TIS Riconosciuta" prompt="Inserire l'importo della CONTRIBUZIONE TIS Riconosciuta (espresso in 2 cifre decimali)" sqref="M6:M1048576 M2:M5" xr:uid="{473EDD48-0FC2-4480-A8CD-51AF57C80278}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei Mensilita Agg. Retr." error="Inserire la quota ratei delle mensilità aggiuntive (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei Mensilita Agg. Retr." prompt="Inserire la quota ratei delle mensilità aggiuntive (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" sqref="N2:N1048576" xr:uid="{54EA3B31-2950-4865-A8E1-E8781022173E}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei Mensilita Agg. Retr." error="Inserire la quota ratei delle mensilità aggiuntive (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei Mensilita Agg. Retr." prompt="Inserire la quota ratei delle mensilità aggiuntive (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" sqref="N6:N1048576 N2:N5" xr:uid="{54EA3B31-2950-4865-A8E1-E8781022173E}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei Mensilita Agg. Contr" error="Inserire la quota ratei per le mensilità aggiuntive (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei Mensilita Agg. Contr" prompt="Inserire la quota ratei per le mensilità aggiuntive (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" sqref="O2:O1048576" xr:uid="{26572884-DABF-4762-A17A-553D66171A2D}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei Mensilita Agg. Contr" error="Inserire la quota ratei per le mensilità aggiuntive (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei Mensilita Agg. Contr" prompt="Inserire la quota ratei per le mensilità aggiuntive (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" sqref="O6:O1048576 O2:O5" xr:uid="{26572884-DABF-4762-A17A-553D66171A2D}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei ROL Perm Ferie" error="Inserire la quota ratei ROL, PERMESSI e FERIE (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei ROL Perm Ferie" prompt="Inserire la quota ratei ROL, PERMESSI e FERIE (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" sqref="P2:P1048576" xr:uid="{9D29FD7A-7F8D-4460-8824-F8103A3B7454}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei ROL Perm Ferie" error="Inserire la quota ratei ROL, PERMESSI e FERIE (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei ROL Perm Ferie" prompt="Inserire la quota ratei ROL, PERMESSI e FERIE (quota RETRIBUTIVA) (espresso in 2 cifre decimali)" sqref="P6:P1048576 P2:P5" xr:uid="{9D29FD7A-7F8D-4460-8824-F8103A3B7454}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei ROL PERM FERIE CONTR" error="Inserire la quota ratei ROL, PERMESSI e FERIE (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei ROL PERM FERIE CONTR" prompt="Inserire la quota ratei ROL, PERMESSI e FERIE (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" sqref="Q2:Q1048576" xr:uid="{E20342BC-F787-4410-B7B8-5F6C66953C46}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Quota Ratei ROL PERM FERIE CONTR" error="Inserire la quota ratei ROL, PERMESSI e FERIE (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" promptTitle="Quota Ratei ROL PERM FERIE CONTR" prompt="Inserire la quota ratei ROL, PERMESSI e FERIE (quota CONTRIBUTIVA) (espresso in 2 cifre decimali)" sqref="Q6:Q1048576 Q2:Q5" xr:uid="{E20342BC-F787-4410-B7B8-5F6C66953C46}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Totale Ore TIS Riconosciute" error="Inserire il numero totale di ore TIS riconosciute al lavoratore per il mese di riferimento (espresso in 2 cifre decimali)" promptTitle="Totale Ore TIS Riconosciute" prompt="Inserire il numero totale di ore TIS riconosciute al lavoratore per il mese di riferimento (espresso in 2 cifre decimali)" sqref="R2:R1048576" xr:uid="{E728BBE3-66EB-4948-BD65-07D8389A9624}">
+    <dataValidation type="decimal" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Totale Ore TIS Riconosciute" error="Inserire il numero totale di ore TIS riconosciute al lavoratore per il mese di riferimento (espresso in 2 cifre decimali)" promptTitle="Totale Ore TIS Riconosciute" prompt="Inserire il numero totale di ore TIS riconosciute al lavoratore per il mese di riferimento (espresso in 2 cifre decimali)" sqref="R6:R1048576 R2:R5" xr:uid="{E728BBE3-66EB-4948-BD65-07D8389A9624}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Divisore Orario Contrattuale" error="Divisore orario contrattuale applicato al lavoratore  (espresso in 2 cifre decimali)" promptTitle="Divisore Orario Contrattuale" prompt="Divisore orario contrattuale applicato al lavoratore  (espresso in 2 cifre decimali)" sqref="W2:W1048576" xr:uid="{56B6BC26-29CF-49D4-9F83-B752F7CE5B19}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Divisore Orario Contrattuale" error="Divisore orario contrattuale applicato al lavoratore  (espresso in 2 cifre decimali)" promptTitle="Divisore Orario Contrattuale" prompt="Divisore orario contrattuale applicato al lavoratore  (espresso in 2 cifre decimali)" sqref="W6:W1048576 W2:W5" xr:uid="{56B6BC26-29CF-49D4-9F83-B752F7CE5B19}">
       <formula1>1</formula1>
       <formula2>220</formula2>
     </dataValidation>
@@ -930,43 +1455,43 @@
           <x14:formula1>
             <xm:f>Istanze!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>A6:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tipologia Contratto" error="Indicare la tipologia del contratto_x000a_TD=Tempo Determinato_x000a_TI=Tempo Indeterminato_x000a_AP=Apprendistato" promptTitle="Tipologia Contratto" prompt="Indicare la tipologia del contratto_x000a_TD=Tempo Determinato_x000a_TI=Tempo Indeterminato_x000a_AP=Apprendistato" xr:uid="{4209DAE6-1DF8-4860-A2CD-75DEDF114DD1}">
           <x14:formula1>
             <xm:f>Tipologiche!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G6:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sgravi aliquota contributiva " error="Vi sono sgravi sull’aliquota contributiva previdenziale del lavoratore? Indicare S o N" promptTitle="Sgravi aliquota contributiva " prompt="Vi sono sgravi sull’aliquota contributiva previdenziale del lavoratore? Indicare S o N" xr:uid="{5E491F2A-CF08-405A-ACBD-CD4BCB1F3C6E}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>J6:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 09/11" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 9 novembre:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" promptTitle="Lavoratore Dip 09/11" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 9 novembre:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" xr:uid="{02DAAFBB-558A-4A95-8FBC-F0E7B8A14749}">
           <x14:formula1>
             <xm:f>Tipologiche!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V1048576</xm:sqref>
+          <xm:sqref>V6:V1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 25/03" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" promptTitle="Lavoratore Dip 25/03" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" xr:uid="{CDB14067-D342-46EF-ADD7-D43F66463AB2}">
           <x14:formula1>
             <xm:f>Tipologiche!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>T2:T1048576</xm:sqref>
+          <xm:sqref>T6:T1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 13/07" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 12 luglio:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" promptTitle="Lavoratore Dip 13/07" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 12 luglio:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" xr:uid="{F0752858-D337-404C-8C61-E24CB378FE5C}">
           <x14:formula1>
             <xm:f>Tipologiche!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U1048576</xm:sqref>
+          <xm:sqref>U6:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 23/02" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" promptTitle="Lavoratore Dip 23/02" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO_x000a_Z = NON APPLICABILE" xr:uid="{7D5DB817-388D-4C6F-990D-4E5B334710B1}">
           <x14:formula1>
             <xm:f>Tipologiche!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>S2:S1048576</xm:sqref>
+          <xm:sqref>S6:S1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -976,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861E526C-F842-4CA2-AE86-3C3CCBFAC172}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1003,8 +1528,260 @@
         <v>26</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="2">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="2">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D11" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D12" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D13" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="2">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="2">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="2">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="2">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D18" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="GCbIAsr8eS4O/CdNCrYvx2AKQspNRh2QrQ7GDupUPm8CRqmb8TL7gNqcNEIN9GIyaXtMJxDzi4kfLrKV1iaOGg==" saltValue="XhiDTMg0p31FHsvJtMDjXQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <dataValidations count="3">
     <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Anno riferimento " error="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2020)" promptTitle="Anno riferimento " prompt="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2020)" sqref="C2:C1048576" xr:uid="{7D64DC23-DD90-4842-A22A-F55D04ACAC42}">
@@ -1026,7 +1803,7 @@
           <x14:formula1>
             <xm:f>Istanze!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>A20:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>